<commit_message>
ajuste requisitos teste para mock
</commit_message>
<xml_diff>
--- a/requisitos/Circuito Tere Verde Requisitos.xlsx
+++ b/requisitos/Circuito Tere Verde Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS\Producao\Circuito_Tere_Verde\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB77CA3-DCA3-4A7D-A57E-09A8CAC377E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4AE0C8-7664-4771-95F1-FB4A2834DC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t>Código</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>RF15</t>
+  </si>
+  <si>
+    <t>Biaxa</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -427,9 +430,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -439,9 +439,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -458,33 +476,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -793,337 +784,337 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="90.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="90.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="22"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="22"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="22"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="22"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1143,182 +1134,182 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="90.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="8" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>